<commit_message>
add general set analyst
</commit_message>
<xml_diff>
--- a/data_set/2_04_mqtt.xlsx
+++ b/data_set/2_04_mqtt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mavramenko\Desktop\magisrt\april\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_projects\mqtt_traffic_research\data_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -4866,11 +4866,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>